<commit_message>
"Adicionados balanços concatenados em uma única planilha."
</commit_message>
<xml_diff>
--- a/Data_frame/balancos_definitivos/AMBV3.xlsx
+++ b/Data_frame/balancos_definitivos/AMBV3.xlsx
@@ -10927,7 +10927,7 @@
         <v>5699514.88</v>
       </c>
       <c r="Y57" t="n">
-        <v>8456794.112</v>
+        <v>8456794.624</v>
       </c>
       <c r="Z57" t="n">
         <v>6793738.24</v>
@@ -10939,7 +10939,7 @@
         <v>6936502.784</v>
       </c>
       <c r="AC57" t="n">
-        <v>8642084.864</v>
+        <v>8642083.84</v>
       </c>
       <c r="AD57" t="n">
         <v>7462778.88</v>
@@ -10951,7 +10951,7 @@
         <v>7820171.776</v>
       </c>
       <c r="AG57" t="n">
-        <v>9867098.112</v>
+        <v>9867097.088</v>
       </c>
       <c r="AH57" t="n">
         <v>8615175.168</v>
@@ -10975,7 +10975,7 @@
         <v>9178456.063999999</v>
       </c>
       <c r="AO57" t="n">
-        <v>12515201.024</v>
+        <v>12515202.048</v>
       </c>
       <c r="AP57" t="n">
         <v>6344508.928</v>
@@ -10998,42 +10998,18 @@
       <c r="AV57" t="n">
         <v>6345336.832</v>
       </c>
-      <c r="AW57" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX57" t="n">
-        <v>0</v>
-      </c>
-      <c r="AY57" t="n">
-        <v>0</v>
-      </c>
-      <c r="AZ57" t="n">
-        <v>0</v>
-      </c>
-      <c r="BA57" t="n">
-        <v>0</v>
-      </c>
-      <c r="BB57" t="n">
-        <v>0</v>
-      </c>
-      <c r="BC57" t="n">
-        <v>0</v>
-      </c>
-      <c r="BD57" t="n">
-        <v>0</v>
-      </c>
-      <c r="BE57" t="n">
-        <v>0</v>
-      </c>
-      <c r="BF57" t="n">
-        <v>0</v>
-      </c>
-      <c r="BG57" t="n">
-        <v>0</v>
-      </c>
-      <c r="BH57" t="n">
-        <v>0</v>
-      </c>
+      <c r="AW57" t="inlineStr"/>
+      <c r="AX57" t="inlineStr"/>
+      <c r="AY57" t="inlineStr"/>
+      <c r="AZ57" t="inlineStr"/>
+      <c r="BA57" t="inlineStr"/>
+      <c r="BB57" t="inlineStr"/>
+      <c r="BC57" t="inlineStr"/>
+      <c r="BD57" t="inlineStr"/>
+      <c r="BE57" t="inlineStr"/>
+      <c r="BF57" t="inlineStr"/>
+      <c r="BG57" t="inlineStr"/>
+      <c r="BH57" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -11107,7 +11083,7 @@
         <v>-2748546.048</v>
       </c>
       <c r="Y58" t="n">
-        <v>-3953172.992</v>
+        <v>-3953172.736</v>
       </c>
       <c r="Z58" t="n">
         <v>-3098147.072</v>
@@ -11119,7 +11095,7 @@
         <v>-3026176</v>
       </c>
       <c r="AC58" t="n">
-        <v>-3993736.192</v>
+        <v>-3993735.68</v>
       </c>
       <c r="AD58" t="n">
         <v>-3493056</v>
@@ -11143,7 +11119,7 @@
         <v>-4028005.888</v>
       </c>
       <c r="AK58" t="n">
-        <v>-5648539.648</v>
+        <v>-5648540.16</v>
       </c>
       <c r="AL58" t="n">
         <v>-4271618.048</v>
@@ -11178,42 +11154,18 @@
       <c r="AV58" t="n">
         <v>-3342304</v>
       </c>
-      <c r="AW58" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX58" t="n">
-        <v>0</v>
-      </c>
-      <c r="AY58" t="n">
-        <v>0</v>
-      </c>
-      <c r="AZ58" t="n">
-        <v>0</v>
-      </c>
-      <c r="BA58" t="n">
-        <v>0</v>
-      </c>
-      <c r="BB58" t="n">
-        <v>0</v>
-      </c>
-      <c r="BC58" t="n">
-        <v>0</v>
-      </c>
-      <c r="BD58" t="n">
-        <v>0</v>
-      </c>
-      <c r="BE58" t="n">
-        <v>0</v>
-      </c>
-      <c r="BF58" t="n">
-        <v>0</v>
-      </c>
-      <c r="BG58" t="n">
-        <v>0</v>
-      </c>
-      <c r="BH58" t="n">
-        <v>0</v>
-      </c>
+      <c r="AW58" t="inlineStr"/>
+      <c r="AX58" t="inlineStr"/>
+      <c r="AY58" t="inlineStr"/>
+      <c r="AZ58" t="inlineStr"/>
+      <c r="BA58" t="inlineStr"/>
+      <c r="BB58" t="inlineStr"/>
+      <c r="BC58" t="inlineStr"/>
+      <c r="BD58" t="inlineStr"/>
+      <c r="BE58" t="inlineStr"/>
+      <c r="BF58" t="inlineStr"/>
+      <c r="BG58" t="inlineStr"/>
+      <c r="BH58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -11275,7 +11227,7 @@
         <v>2020881.024</v>
       </c>
       <c r="U59" t="n">
-        <v>2809901.056</v>
+        <v>2809900.8</v>
       </c>
       <c r="V59" t="n">
         <v>2370492.928</v>
@@ -11299,7 +11251,7 @@
         <v>3910327.04</v>
       </c>
       <c r="AC59" t="n">
-        <v>4648347.648</v>
+        <v>4648346.624</v>
       </c>
       <c r="AD59" t="n">
         <v>3969722.88</v>
@@ -11323,7 +11275,7 @@
         <v>4641717.76</v>
       </c>
       <c r="AK59" t="n">
-        <v>5826447.36</v>
+        <v>5826446.336</v>
       </c>
       <c r="AL59" t="n">
         <v>4847789.056</v>
@@ -11371,7 +11323,7 @@
         <v>6374534.144</v>
       </c>
       <c r="BA59" t="n">
-        <v>8378443.776</v>
+        <v>8378442.24</v>
       </c>
       <c r="BB59" t="n">
         <v>7235714.048</v>
@@ -11383,7 +11335,7 @@
         <v>8036021.76</v>
       </c>
       <c r="BE59" t="n">
-        <v>10133891.072</v>
+        <v>10133890.048</v>
       </c>
       <c r="BF59" t="n">
         <v>7772806.144</v>
@@ -11491,7 +11443,7 @@
         <v>-1479532.032</v>
       </c>
       <c r="AG60" t="n">
-        <v>-1795960.832</v>
+        <v>-1795960.704</v>
       </c>
       <c r="AH60" t="n">
         <v>-1551965.056</v>
@@ -11503,7 +11455,7 @@
         <v>-1544993.024</v>
       </c>
       <c r="AK60" t="n">
-        <v>-1887737.856</v>
+        <v>-1887737.984</v>
       </c>
       <c r="AL60" t="n">
         <v>-1644840.96</v>
@@ -11515,7 +11467,7 @@
         <v>-1682089.984</v>
       </c>
       <c r="AO60" t="n">
-        <v>-2201872.896</v>
+        <v>-2201873.152</v>
       </c>
       <c r="AP60" t="n">
         <v>-1052019.968</v>
@@ -11563,7 +11515,7 @@
         <v>-2621932.032</v>
       </c>
       <c r="BE60" t="n">
-        <v>-3056449.536</v>
+        <v>-3056449.28</v>
       </c>
       <c r="BF60" t="n">
         <v>-2622822.912</v>
@@ -11671,7 +11623,7 @@
         <v>2857786.88</v>
       </c>
       <c r="AG61" t="n">
-        <v>3473515.52</v>
+        <v>3473515.008</v>
       </c>
       <c r="AH61" t="n">
         <v>3103036.928</v>
@@ -11683,7 +11635,7 @@
         <v>3096724.992</v>
       </c>
       <c r="AK61" t="n">
-        <v>3938708.48</v>
+        <v>3938708.736</v>
       </c>
       <c r="AL61" t="n">
         <v>3202948.096</v>
@@ -11695,7 +11647,7 @@
         <v>3127813.12</v>
       </c>
       <c r="AO61" t="n">
-        <v>4300454.912</v>
+        <v>4300455.424</v>
       </c>
       <c r="AP61" t="n">
         <v>1650130.944</v>
@@ -11743,7 +11695,7 @@
         <v>5414090.24</v>
       </c>
       <c r="BE61" t="n">
-        <v>7077437.44</v>
+        <v>7077436.928</v>
       </c>
       <c r="BF61" t="n">
         <v>5149983.232</v>
@@ -11815,7 +11767,7 @@
         <v>-336336</v>
       </c>
       <c r="U62" t="n">
-        <v>-534396.928</v>
+        <v>-534396.96</v>
       </c>
       <c r="V62" t="n">
         <v>-449955.008</v>
@@ -11851,7 +11803,7 @@
         <v>-950396.032</v>
       </c>
       <c r="AG62" t="n">
-        <v>-1057344.768</v>
+        <v>-1057344.896</v>
       </c>
       <c r="AH62" t="n">
         <v>-989838.0159999999</v>
@@ -11923,7 +11875,7 @@
         <v>-1820696.96</v>
       </c>
       <c r="BE62" t="n">
-        <v>-1974976</v>
+        <v>-1974976.256</v>
       </c>
       <c r="BF62" t="n">
         <v>-1988907.008</v>
@@ -12019,7 +11971,7 @@
         <v>-481689.984</v>
       </c>
       <c r="AC63" t="n">
-        <v>-518061.952</v>
+        <v>-518061.984</v>
       </c>
       <c r="AD63" t="n">
         <v>-443571.008</v>
@@ -12031,7 +11983,7 @@
         <v>-536148</v>
       </c>
       <c r="AG63" t="n">
-        <v>-31423.872</v>
+        <v>-31423.968</v>
       </c>
       <c r="AH63" t="n">
         <v>-398886.016</v>
@@ -12079,7 +12031,7 @@
         <v>-236444.992</v>
       </c>
       <c r="AW63" t="n">
-        <v>-481449.088</v>
+        <v>-481449.056</v>
       </c>
       <c r="AX63" t="n">
         <v>-322644</v>
@@ -12091,7 +12043,7 @@
         <v>-278384</v>
       </c>
       <c r="BA63" t="n">
-        <v>-369940.992</v>
+        <v>-369941.024</v>
       </c>
       <c r="BB63" t="n">
         <v>-303611.008</v>
@@ -12103,7 +12055,7 @@
         <v>-504852.992</v>
       </c>
       <c r="BE63" t="n">
-        <v>-395064.064</v>
+        <v>-395064.032</v>
       </c>
       <c r="BF63" t="n">
         <v>-351740</v>
@@ -12138,99 +12090,37 @@
       <c r="P64" t="inlineStr"/>
       <c r="Q64" t="inlineStr"/>
       <c r="R64" t="inlineStr"/>
-      <c r="S64" t="n">
-        <v>0</v>
-      </c>
-      <c r="T64" t="n">
-        <v>0</v>
-      </c>
-      <c r="U64" t="n">
-        <v>0</v>
-      </c>
-      <c r="V64" t="n">
-        <v>0</v>
-      </c>
-      <c r="W64" t="n">
-        <v>0</v>
-      </c>
-      <c r="X64" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y64" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z64" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA64" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB64" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC64" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD64" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE64" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF64" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG64" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH64" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI64" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ64" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK64" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL64" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM64" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN64" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO64" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP64" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ64" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR64" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS64" t="n">
-        <v>0</v>
-      </c>
-      <c r="AT64" t="n">
-        <v>0</v>
-      </c>
-      <c r="AU64" t="n">
-        <v>0</v>
-      </c>
-      <c r="AV64" t="n">
-        <v>0</v>
-      </c>
-      <c r="AW64" t="n">
-        <v>0</v>
-      </c>
+      <c r="S64" t="inlineStr"/>
+      <c r="T64" t="inlineStr"/>
+      <c r="U64" t="inlineStr"/>
+      <c r="V64" t="inlineStr"/>
+      <c r="W64" t="inlineStr"/>
+      <c r="X64" t="inlineStr"/>
+      <c r="Y64" t="inlineStr"/>
+      <c r="Z64" t="inlineStr"/>
+      <c r="AA64" t="inlineStr"/>
+      <c r="AB64" t="inlineStr"/>
+      <c r="AC64" t="inlineStr"/>
+      <c r="AD64" t="inlineStr"/>
+      <c r="AE64" t="inlineStr"/>
+      <c r="AF64" t="inlineStr"/>
+      <c r="AG64" t="inlineStr"/>
+      <c r="AH64" t="inlineStr"/>
+      <c r="AI64" t="inlineStr"/>
+      <c r="AJ64" t="inlineStr"/>
+      <c r="AK64" t="inlineStr"/>
+      <c r="AL64" t="inlineStr"/>
+      <c r="AM64" t="inlineStr"/>
+      <c r="AN64" t="inlineStr"/>
+      <c r="AO64" t="inlineStr"/>
+      <c r="AP64" t="inlineStr"/>
+      <c r="AQ64" t="inlineStr"/>
+      <c r="AR64" t="inlineStr"/>
+      <c r="AS64" t="inlineStr"/>
+      <c r="AT64" t="inlineStr"/>
+      <c r="AU64" t="inlineStr"/>
+      <c r="AV64" t="inlineStr"/>
+      <c r="AW64" t="inlineStr"/>
       <c r="AX64" t="n">
         <v>0</v>
       </c>
@@ -12337,7 +12227,7 @@
         <v>38592</v>
       </c>
       <c r="Y65" t="n">
-        <v>271743.008</v>
+        <v>271742.976</v>
       </c>
       <c r="Z65" t="n">
         <v>78355</v>
@@ -12349,7 +12239,7 @@
         <v>32538</v>
       </c>
       <c r="AC65" t="n">
-        <v>31853.984</v>
+        <v>31853.976</v>
       </c>
       <c r="AD65" t="n">
         <v>49006</v>
@@ -12361,7 +12251,7 @@
         <v>89564</v>
       </c>
       <c r="AG65" t="n">
-        <v>112683.984</v>
+        <v>112683.992</v>
       </c>
       <c r="AH65" t="n">
         <v>57173</v>
@@ -12397,7 +12287,7 @@
         <v>241952.992</v>
       </c>
       <c r="AS65" t="n">
-        <v>-47865.024</v>
+        <v>-47864.992</v>
       </c>
       <c r="AT65" t="n">
         <v>147732</v>
@@ -12505,7 +12395,7 @@
         <v>-89349</v>
       </c>
       <c r="U66" t="n">
-        <v>-69702.976</v>
+        <v>-69702.992</v>
       </c>
       <c r="V66" t="n">
         <v>-74930</v>
@@ -12529,7 +12419,7 @@
         <v>-344040</v>
       </c>
       <c r="AC66" t="n">
-        <v>-202403.968</v>
+        <v>-202404.032</v>
       </c>
       <c r="AD66" t="n">
         <v>-295041.984</v>
@@ -12757,7 +12647,7 @@
         <v>532203.008</v>
       </c>
       <c r="AS67" t="n">
-        <v>-1280947.072</v>
+        <v>-1280946.944</v>
       </c>
       <c r="AT67" t="n">
         <v>906222.976</v>
@@ -12877,7 +12767,7 @@
         <v>-138614</v>
       </c>
       <c r="Y68" t="n">
-        <v>-220592.96</v>
+        <v>-220592.976</v>
       </c>
       <c r="Z68" t="n">
         <v>-275192.992</v>
@@ -12889,7 +12779,7 @@
         <v>-242163.008</v>
       </c>
       <c r="AC68" t="n">
-        <v>-318374.912</v>
+        <v>-318374.944</v>
       </c>
       <c r="AD68" t="n">
         <v>-170414</v>
@@ -12925,7 +12815,7 @@
         <v>-286392</v>
       </c>
       <c r="AO68" t="n">
-        <v>-199520</v>
+        <v>-199520.032</v>
       </c>
       <c r="AP68" t="n">
         <v>-156560</v>
@@ -12961,7 +12851,7 @@
         <v>-306340</v>
       </c>
       <c r="BA68" t="n">
-        <v>-90980.992</v>
+        <v>-90981</v>
       </c>
       <c r="BB68" t="n">
         <v>-59997</v>
@@ -12973,7 +12863,7 @@
         <v>-344272</v>
       </c>
       <c r="BE68" t="n">
-        <v>-240225.984</v>
+        <v>-240226.016</v>
       </c>
       <c r="BF68" t="n">
         <v>-240687.008</v>
@@ -13045,7 +12935,7 @@
         <v>152770</v>
       </c>
       <c r="U69" t="n">
-        <v>46517.056</v>
+        <v>46517.032</v>
       </c>
       <c r="V69" t="n">
         <v>112848</v>
@@ -13057,7 +12947,7 @@
         <v>-46106</v>
       </c>
       <c r="Y69" t="n">
-        <v>-57787.968</v>
+        <v>-57787.984</v>
       </c>
       <c r="Z69" t="n">
         <v>42831</v>
@@ -13129,7 +13019,7 @@
         <v>293585.984</v>
       </c>
       <c r="AW69" t="n">
-        <v>291058.048</v>
+        <v>291058.016</v>
       </c>
       <c r="AX69" t="n">
         <v>228872.992</v>
@@ -13153,7 +13043,7 @@
         <v>183866</v>
       </c>
       <c r="BE69" t="n">
-        <v>146062.048</v>
+        <v>146062.032</v>
       </c>
       <c r="BF69" t="n">
         <v>160687.008</v>
@@ -13225,7 +13115,7 @@
         <v>-261476</v>
       </c>
       <c r="U70" t="n">
-        <v>-250804</v>
+        <v>-250803.984</v>
       </c>
       <c r="V70" t="n">
         <v>-328660.992</v>
@@ -13273,7 +13163,7 @@
         <v>-340452</v>
       </c>
       <c r="AK70" t="n">
-        <v>-348231.04</v>
+        <v>-348231.008</v>
       </c>
       <c r="AL70" t="n">
         <v>-343601.984</v>
@@ -13285,7 +13175,7 @@
         <v>-659792</v>
       </c>
       <c r="AO70" t="n">
-        <v>-468635.008</v>
+        <v>-468635.072</v>
       </c>
       <c r="AP70" t="n">
         <v>-386284.992</v>
@@ -13297,7 +13187,7 @@
         <v>-406336.992</v>
       </c>
       <c r="AS70" t="n">
-        <v>108771.072</v>
+        <v>108770.976</v>
       </c>
       <c r="AT70" t="n">
         <v>-283860</v>
@@ -13321,7 +13211,7 @@
         <v>-450400</v>
       </c>
       <c r="BA70" t="n">
-        <v>-239116.928</v>
+        <v>-239116.96</v>
       </c>
       <c r="BB70" t="n">
         <v>-267942</v>
@@ -13429,7 +13319,7 @@
         <v>-6364</v>
       </c>
       <c r="AC71" t="n">
-        <v>-60903.984</v>
+        <v>-60903.992</v>
       </c>
       <c r="AD71" t="n">
         <v>4755</v>
@@ -13488,42 +13378,18 @@
       <c r="AV71" t="n">
         <v>0</v>
       </c>
-      <c r="AW71" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX71" t="n">
-        <v>0</v>
-      </c>
-      <c r="AY71" t="n">
-        <v>0</v>
-      </c>
-      <c r="AZ71" t="n">
-        <v>0</v>
-      </c>
-      <c r="BA71" t="n">
-        <v>0</v>
-      </c>
-      <c r="BB71" t="n">
-        <v>0</v>
-      </c>
-      <c r="BC71" t="n">
-        <v>0</v>
-      </c>
-      <c r="BD71" t="n">
-        <v>0</v>
-      </c>
-      <c r="BE71" t="n">
-        <v>0</v>
-      </c>
-      <c r="BF71" t="n">
-        <v>0</v>
-      </c>
-      <c r="BG71" t="n">
-        <v>0</v>
-      </c>
-      <c r="BH71" t="n">
-        <v>0</v>
-      </c>
+      <c r="AW71" t="inlineStr"/>
+      <c r="AX71" t="inlineStr"/>
+      <c r="AY71" t="inlineStr"/>
+      <c r="AZ71" t="inlineStr"/>
+      <c r="BA71" t="inlineStr"/>
+      <c r="BB71" t="inlineStr"/>
+      <c r="BC71" t="inlineStr"/>
+      <c r="BD71" t="inlineStr"/>
+      <c r="BE71" t="inlineStr"/>
+      <c r="BF71" t="inlineStr"/>
+      <c r="BG71" t="inlineStr"/>
+      <c r="BH71" t="inlineStr"/>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -13668,42 +13534,18 @@
       <c r="AV72" t="n">
         <v>0</v>
       </c>
-      <c r="AW72" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX72" t="n">
-        <v>0</v>
-      </c>
-      <c r="AY72" t="n">
-        <v>0</v>
-      </c>
-      <c r="AZ72" t="n">
-        <v>0</v>
-      </c>
-      <c r="BA72" t="n">
-        <v>0</v>
-      </c>
-      <c r="BB72" t="n">
-        <v>0</v>
-      </c>
-      <c r="BC72" t="n">
-        <v>0</v>
-      </c>
-      <c r="BD72" t="n">
-        <v>0</v>
-      </c>
-      <c r="BE72" t="n">
-        <v>0</v>
-      </c>
-      <c r="BF72" t="n">
-        <v>0</v>
-      </c>
-      <c r="BG72" t="n">
-        <v>0</v>
-      </c>
-      <c r="BH72" t="n">
-        <v>0</v>
-      </c>
+      <c r="AW72" t="inlineStr"/>
+      <c r="AX72" t="inlineStr"/>
+      <c r="AY72" t="inlineStr"/>
+      <c r="AZ72" t="inlineStr"/>
+      <c r="BA72" t="inlineStr"/>
+      <c r="BB72" t="inlineStr"/>
+      <c r="BC72" t="inlineStr"/>
+      <c r="BD72" t="inlineStr"/>
+      <c r="BE72" t="inlineStr"/>
+      <c r="BF72" t="inlineStr"/>
+      <c r="BG72" t="inlineStr"/>
+      <c r="BH72" t="inlineStr"/>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -13789,7 +13631,7 @@
         <v>-37350</v>
       </c>
       <c r="AC73" t="n">
-        <v>-47707.008</v>
+        <v>-47707.016</v>
       </c>
       <c r="AD73" t="n">
         <v>-14843</v>
@@ -13848,42 +13690,18 @@
       <c r="AV73" t="n">
         <v>0</v>
       </c>
-      <c r="AW73" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX73" t="n">
-        <v>0</v>
-      </c>
-      <c r="AY73" t="n">
-        <v>0</v>
-      </c>
-      <c r="AZ73" t="n">
-        <v>0</v>
-      </c>
-      <c r="BA73" t="n">
-        <v>0</v>
-      </c>
-      <c r="BB73" t="n">
-        <v>0</v>
-      </c>
-      <c r="BC73" t="n">
-        <v>0</v>
-      </c>
-      <c r="BD73" t="n">
-        <v>0</v>
-      </c>
-      <c r="BE73" t="n">
-        <v>0</v>
-      </c>
-      <c r="BF73" t="n">
-        <v>0</v>
-      </c>
-      <c r="BG73" t="n">
-        <v>0</v>
-      </c>
-      <c r="BH73" t="n">
-        <v>0</v>
-      </c>
+      <c r="AW73" t="inlineStr"/>
+      <c r="AX73" t="inlineStr"/>
+      <c r="AY73" t="inlineStr"/>
+      <c r="AZ73" t="inlineStr"/>
+      <c r="BA73" t="inlineStr"/>
+      <c r="BB73" t="inlineStr"/>
+      <c r="BC73" t="inlineStr"/>
+      <c r="BD73" t="inlineStr"/>
+      <c r="BE73" t="inlineStr"/>
+      <c r="BF73" t="inlineStr"/>
+      <c r="BG73" t="inlineStr"/>
+      <c r="BH73" t="inlineStr"/>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -13945,7 +13763,7 @@
         <v>418976</v>
       </c>
       <c r="U74" t="n">
-        <v>466145.92</v>
+        <v>466145.984</v>
       </c>
       <c r="V74" t="n">
         <v>420460.992</v>
@@ -13957,7 +13775,7 @@
         <v>304943.008</v>
       </c>
       <c r="Y74" t="n">
-        <v>799721.92</v>
+        <v>799721.9840000001</v>
       </c>
       <c r="Z74" t="n">
         <v>291940</v>
@@ -14005,7 +13823,7 @@
         <v>1305420.032</v>
       </c>
       <c r="AO74" t="n">
-        <v>1510797.824</v>
+        <v>1510798.08</v>
       </c>
       <c r="AP74" t="n">
         <v>1808691.968</v>
@@ -14017,7 +13835,7 @@
         <v>1559699.968</v>
       </c>
       <c r="AS74" t="n">
-        <v>3749697.536</v>
+        <v>3749697.28</v>
       </c>
       <c r="AT74" t="n">
         <v>1816984.96</v>
@@ -14053,7 +13871,7 @@
         <v>2986521.088</v>
       </c>
       <c r="BE74" t="n">
-        <v>4757252.096</v>
+        <v>4757251.584</v>
       </c>
       <c r="BF74" t="n">
         <v>2882859.008</v>
@@ -14137,7 +13955,7 @@
         <v>-113496</v>
       </c>
       <c r="Y75" t="n">
-        <v>-506705.024</v>
+        <v>-506704.992</v>
       </c>
       <c r="Z75" t="n">
         <v>-164236</v>
@@ -14233,7 +14051,7 @@
         <v>-385540</v>
       </c>
       <c r="BE75" t="n">
-        <v>-411236.096</v>
+        <v>-411236.064</v>
       </c>
       <c r="BF75" t="n">
         <v>-768368</v>
@@ -14305,7 +14123,7 @@
         <v>57960</v>
       </c>
       <c r="U76" t="n">
-        <v>44191.008</v>
+        <v>44191</v>
       </c>
       <c r="V76" t="n">
         <v>3888</v>
@@ -14353,7 +14171,7 @@
         <v>-173010</v>
       </c>
       <c r="AK76" t="n">
-        <v>-142744</v>
+        <v>-142743.968</v>
       </c>
       <c r="AL76" t="n">
         <v>-110171</v>
@@ -14568,42 +14386,18 @@
       <c r="AV77" t="n">
         <v>0</v>
       </c>
-      <c r="AW77" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX77" t="n">
-        <v>0</v>
-      </c>
-      <c r="AY77" t="n">
-        <v>0</v>
-      </c>
-      <c r="AZ77" t="n">
-        <v>0</v>
-      </c>
-      <c r="BA77" t="n">
-        <v>0</v>
-      </c>
-      <c r="BB77" t="n">
-        <v>0</v>
-      </c>
-      <c r="BC77" t="n">
-        <v>0</v>
-      </c>
-      <c r="BD77" t="n">
-        <v>0</v>
-      </c>
-      <c r="BE77" t="n">
-        <v>0</v>
-      </c>
-      <c r="BF77" t="n">
-        <v>0</v>
-      </c>
-      <c r="BG77" t="n">
-        <v>0</v>
-      </c>
-      <c r="BH77" t="n">
-        <v>0</v>
-      </c>
+      <c r="AW77" t="inlineStr"/>
+      <c r="AX77" t="inlineStr"/>
+      <c r="AY77" t="inlineStr"/>
+      <c r="AZ77" t="inlineStr"/>
+      <c r="BA77" t="inlineStr"/>
+      <c r="BB77" t="inlineStr"/>
+      <c r="BC77" t="inlineStr"/>
+      <c r="BD77" t="inlineStr"/>
+      <c r="BE77" t="inlineStr"/>
+      <c r="BF77" t="inlineStr"/>
+      <c r="BG77" t="inlineStr"/>
+      <c r="BH77" t="inlineStr"/>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -14748,42 +14542,18 @@
       <c r="AV78" t="n">
         <v>0</v>
       </c>
-      <c r="AW78" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX78" t="n">
-        <v>0</v>
-      </c>
-      <c r="AY78" t="n">
-        <v>0</v>
-      </c>
-      <c r="AZ78" t="n">
-        <v>0</v>
-      </c>
-      <c r="BA78" t="n">
-        <v>0</v>
-      </c>
-      <c r="BB78" t="n">
-        <v>0</v>
-      </c>
-      <c r="BC78" t="n">
-        <v>0</v>
-      </c>
-      <c r="BD78" t="n">
-        <v>0</v>
-      </c>
-      <c r="BE78" t="n">
-        <v>0</v>
-      </c>
-      <c r="BF78" t="n">
-        <v>0</v>
-      </c>
-      <c r="BG78" t="n">
-        <v>0</v>
-      </c>
-      <c r="BH78" t="n">
-        <v>0</v>
-      </c>
+      <c r="AW78" t="inlineStr"/>
+      <c r="AX78" t="inlineStr"/>
+      <c r="AY78" t="inlineStr"/>
+      <c r="AZ78" t="inlineStr"/>
+      <c r="BA78" t="inlineStr"/>
+      <c r="BB78" t="inlineStr"/>
+      <c r="BC78" t="inlineStr"/>
+      <c r="BD78" t="inlineStr"/>
+      <c r="BE78" t="inlineStr"/>
+      <c r="BF78" t="inlineStr"/>
+      <c r="BG78" t="inlineStr"/>
+      <c r="BH78" t="inlineStr"/>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -14905,30 +14675,14 @@
       <c r="AO79" t="n">
         <v>-15117</v>
       </c>
-      <c r="AP79" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ79" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR79" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS79" t="n">
-        <v>0</v>
-      </c>
-      <c r="AT79" t="n">
-        <v>0</v>
-      </c>
-      <c r="AU79" t="n">
-        <v>0</v>
-      </c>
-      <c r="AV79" t="n">
-        <v>0</v>
-      </c>
-      <c r="AW79" t="n">
-        <v>0</v>
-      </c>
+      <c r="AP79" t="inlineStr"/>
+      <c r="AQ79" t="inlineStr"/>
+      <c r="AR79" t="inlineStr"/>
+      <c r="AS79" t="inlineStr"/>
+      <c r="AT79" t="inlineStr"/>
+      <c r="AU79" t="inlineStr"/>
+      <c r="AV79" t="inlineStr"/>
+      <c r="AW79" t="inlineStr"/>
       <c r="AX79" t="n">
         <v>-17366</v>
       </c>
@@ -15047,7 +14801,7 @@
         <v>399081.984</v>
       </c>
       <c r="AC80" t="n">
-        <v>697188.096</v>
+        <v>697188.032</v>
       </c>
       <c r="AD80" t="n">
         <v>655899.008</v>
@@ -15083,7 +14837,7 @@
         <v>949036.032</v>
       </c>
       <c r="AO80" t="n">
-        <v>964534.912</v>
+        <v>964534.976</v>
       </c>
       <c r="AP80" t="n">
         <v>1539315.968</v>

</xml_diff>